<commit_message>
Added loading of the datasets
</commit_message>
<xml_diff>
--- a/resources/lidar-2022.xlsx
+++ b/resources/lidar-2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/ashtanm1_student_ubc_ca/Documents/School/2023S/minecraftUBC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/ashtanm1_student_ubc_ca/Documents/School/2023S/minecraftUBC/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="4" documentId="11_B55C422FC0D1856F8CE00460188020FE91837AF7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D9FBC11-B498-478E-BE86-74A4803ED53A}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1095" yWindow="10605" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2503,7 +2503,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>